<commit_message>
arrow + bugfix plank
</commit_message>
<xml_diff>
--- a/stuklijst.xlsx
+++ b/stuklijst.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,10 +492,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>74</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -503,7 +503,7 @@
       <c r="B3" s="1" t="n"/>
       <c r="C3" s="1" t="n"/>
       <c r="D3" s="1" t="n">
-        <v>80</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="E3" t="n">
         <v>6</v>
@@ -514,10 +514,10 @@
       <c r="B4" s="1" t="n"/>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="1" t="n">
-        <v>113.3</v>
+        <v>93.3</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -525,7 +525,7 @@
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n">
-        <v>239.6</v>
+        <v>184.6</v>
       </c>
       <c r="E5" t="n">
         <v>6</v>
@@ -563,7 +563,7 @@
         <v>7.5</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>250</v>
+        <v>195</v>
       </c>
       <c r="E7" t="n">
         <v>3</v>
@@ -576,7 +576,7 @@
         <v>14.1</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>250</v>
+        <v>195</v>
       </c>
       <c r="E8" t="n">
         <v>4</v>
@@ -586,26 +586,26 @@
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="n"/>
       <c r="C9" s="1" t="n">
-        <v>17</v>
+        <v>14.8</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>234.6</v>
+        <v>194.6</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="n"/>
       <c r="C10" s="1" t="n">
-        <v>20</v>
+        <v>17.8</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>97.40000000000001</v>
+        <v>195</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -613,21 +613,23 @@
       <c r="B11" s="1" t="n"/>
       <c r="C11" s="1" t="n"/>
       <c r="D11" s="1" t="n">
-        <v>234.6</v>
+        <v>195.6</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="n"/>
-      <c r="C12" s="1" t="n"/>
+      <c r="C12" s="1" t="n">
+        <v>20</v>
+      </c>
       <c r="D12" s="1" t="n">
-        <v>235.6</v>
+        <v>79.40000000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -635,58 +637,81 @@
       <c r="B13" s="1" t="n"/>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="n">
-        <v>250</v>
+        <v>194.6</v>
       </c>
       <c r="E13" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="1" t="n"/>
+      <c r="C14" s="1" t="n"/>
+      <c r="D14" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="E14" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="n"/>
+      <c r="C15" s="1" t="n"/>
+      <c r="D15" s="1" t="n">
+        <v>195.6</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>scharnier</t>
         </is>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C16" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D16" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E16" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
         <is>
           <t>slot</t>
         </is>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C17" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D17" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E17" t="n">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="A7:A15"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="B7:B15"/>
     <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
arrow label and camera
</commit_message>
<xml_diff>
--- a/stuklijst.xlsx
+++ b/stuklijst.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,10 +492,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>69.59999999999999</v>
+        <v>39.6</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -503,10 +503,10 @@
       <c r="B3" s="1" t="n"/>
       <c r="C3" s="1" t="n"/>
       <c r="D3" s="1" t="n">
-        <v>75.59999999999999</v>
+        <v>45.6</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -514,7 +514,7 @@
       <c r="B4" s="1" t="n"/>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="1" t="n">
-        <v>93.3</v>
+        <v>84.59999999999999</v>
       </c>
       <c r="E4" t="n">
         <v>4</v>
@@ -525,10 +525,10 @@
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n">
-        <v>184.6</v>
+        <v>89.59999999999999</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -547,7 +547,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -563,33 +563,33 @@
         <v>7.5</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>195</v>
+        <v>95</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="n">
-        <v>14.1</v>
+        <v>12.2</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>195</v>
+        <v>95</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="n"/>
       <c r="C9" s="1" t="n">
-        <v>14.8</v>
+        <v>12.8</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>194.6</v>
+        <v>95</v>
       </c>
       <c r="E9" t="n">
         <v>4</v>
@@ -598,11 +598,9 @@
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="n">
-        <v>17.8</v>
-      </c>
+      <c r="C10" s="1" t="n"/>
       <c r="D10" s="1" t="n">
-        <v>195</v>
+        <v>95.59999999999999</v>
       </c>
       <c r="E10" t="n">
         <v>4</v>
@@ -611,9 +609,11 @@
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="n"/>
-      <c r="C11" s="1" t="n"/>
+      <c r="C11" s="1" t="n">
+        <v>19.8</v>
+      </c>
       <c r="D11" s="1" t="n">
-        <v>195.6</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="E11" t="n">
         <v>4</v>
@@ -626,10 +626,10 @@
         <v>20</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>79.40000000000001</v>
+        <v>76</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -637,10 +637,10 @@
       <c r="B13" s="1" t="n"/>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="n">
-        <v>194.6</v>
+        <v>95</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -648,70 +648,59 @@
       <c r="B14" s="1" t="n"/>
       <c r="C14" s="1" t="n"/>
       <c r="D14" s="1" t="n">
-        <v>195</v>
+        <v>95.59999999999999</v>
       </c>
       <c r="E14" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n"/>
-      <c r="B15" s="1" t="n"/>
-      <c r="C15" s="1" t="n"/>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>scharnier</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>10</v>
+      </c>
       <c r="D15" s="1" t="n">
-        <v>195.6</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>scharnier</t>
+          <t>slot</t>
         </is>
       </c>
       <c r="B16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>slot</t>
-        </is>
-      </c>
-      <c r="B17" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="E17" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A15"/>
+    <mergeCell ref="A7:A14"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="B7:B14"/>
     <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>